<commit_message>
update new test case for ClickAction page
</commit_message>
<xml_diff>
--- a/Test_Data.xlsx
+++ b/Test_Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\00_MASTER OF COMPUTER SCIENCE_MUM\00_Projects\19_WebDriverUniversity_POM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E7C2726-4D1E-435C-B882-21BEDABB7250}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD0B74CB-C988-402F-945E-EBD0D5BA8792}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
   <si>
     <t>Username</t>
   </si>
@@ -58,23 +58,70 @@
     <t>comment</t>
   </si>
   <si>
-    <t>function</t>
-  </si>
-  <si>
-    <t>submit</t>
-  </si>
-  <si>
-    <t>reset</t>
+    <t>Bao</t>
+  </si>
+  <si>
+    <t>Nguyen</t>
+  </si>
+  <si>
+    <t>abc@gmail.com</t>
+  </si>
+  <si>
+    <t>Note1</t>
+  </si>
+  <si>
+    <t>Note2</t>
+  </si>
+  <si>
+    <t>Note3</t>
+  </si>
+  <si>
+    <t>Note4</t>
+  </si>
+  <si>
+    <t>Note5</t>
+  </si>
+  <si>
+    <t>123&amp;**</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>Note7</t>
+  </si>
+  <si>
+    <t>*&amp;^^()!</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>Submit - Expected Result</t>
+  </si>
+  <si>
+    <t>Submit - Actual Result</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -97,13 +144,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -382,15 +432,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -404,20 +462,132 @@
         <v>9</v>
       </c>
       <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
       <c r="E2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
       <c r="E3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>12239</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{E02BF80F-244D-4C76-8A1C-654C6E36A097}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{1091D46D-C184-42A0-8A8E-948931EF6B66}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{BF371FE6-B304-4BD4-8028-F7C1240D0FC5}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{C3454AAF-724E-41FC-8BF6-FA170B0D3878}"/>
+    <hyperlink ref="C7" r:id="rId5" xr:uid="{B4A5CDEC-ADFF-498D-87BC-B5B371F6B306}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
new TodoList page added
</commit_message>
<xml_diff>
--- a/Test_Data.xlsx
+++ b/Test_Data.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\00_MASTER OF COMPUTER SCIENCE_MUM\00_Projects\19_WebDriverUniversity_POM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD0B74CB-C988-402F-945E-EBD0D5BA8792}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E23EC633-3747-49F5-B93D-E43B661B1968}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ContactUs" sheetId="1" r:id="rId1"/>
-    <sheet name="Login" sheetId="2" r:id="rId2"/>
+    <sheet name="ToDoItems" sheetId="3" r:id="rId2"/>
+    <sheet name="Login" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
   <si>
     <t>Username</t>
   </si>
@@ -104,6 +105,18 @@
   </si>
   <si>
     <t>Submit - Actual Result</t>
+  </si>
+  <si>
+    <t>items</t>
+  </si>
+  <si>
+    <t>1. new item 1</t>
+  </si>
+  <si>
+    <t>new item 2</t>
+  </si>
+  <si>
+    <t>new &amp;&amp;!*@</t>
   </si>
 </sst>
 </file>
@@ -434,7 +447,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -593,6 +606,46 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{153BBF7E-33D9-4FE9-9D63-29CD8197CDB4}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08ED881-F58D-4410-BDA3-FF357C53318E}">
   <dimension ref="A1:B4"/>
   <sheetViews>

</xml_diff>